<commit_message>
add layers for MCA
</commit_message>
<xml_diff>
--- a/data_source_and_MCA_criteria.xlsx
+++ b/data_source_and_MCA_criteria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ck\workspace\GIS\gis_analysis_hamburg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609B9E55-45DF-42F3-A3B2-529D7BD4C382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3897C3-9CD5-4FC9-8C9F-BEFFA87B52F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CCC0EF6C-A448-42CE-850E-28F2528C25EE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
   <si>
     <t>Data Source</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -185,6 +185,24 @@
   <si>
     <t>Protected Planet</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wind Speed at 100m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://globalwindatlas.info/en</t>
+  </si>
+  <si>
+    <t>Global Wind Atlas</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OSM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://download.geofabrik.de/europe/germany/hamburg.html</t>
   </si>
 </sst>
 </file>
@@ -570,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB44F095-CA0A-40F6-96CD-B28484F14A6A}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -629,27 +647,68 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
         <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -665,15 +724,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB75600-C524-4091-8455-43029D226ECA}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.3984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.3984375" customWidth="1"/>
     <col min="6" max="6" width="12.796875" bestFit="1" customWidth="1"/>
@@ -796,6 +855,14 @@
         <v>27</v>
       </c>
     </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update MCA data source
</commit_message>
<xml_diff>
--- a/data_source_and_MCA_criteria.xlsx
+++ b/data_source_and_MCA_criteria.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ck\workspace\GIS\gis_analysis_hamburg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F733DD9-C0C7-4188-B20A-40F629DB6458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CDD07CA-FCE4-45B4-9E19-8716B5988461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CCC0EF6C-A448-42CE-850E-28F2528C25EE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
   <si>
     <t>Data Source</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -198,11 +198,34 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>OSM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://download.geofabrik.de/europe/germany/hamburg.html</t>
+    <t>Exclusive Range</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://gee-community-catalog.org/projects/energy_farms/?h=wind+farm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vector</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://gee-community-catalog.org/projects/grip/?h=roads</t>
+  </si>
+  <si>
+    <t>Bathymetry</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GEE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GEE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://gee-community-catalog.org/projects/globathy/?h=globath</t>
   </si>
 </sst>
 </file>
@@ -292,9 +315,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 테마">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -332,7 +355,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -438,7 +461,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -580,7 +603,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -591,7 +614,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -658,13 +681,13 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
@@ -672,21 +695,19 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>41</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
@@ -694,22 +715,14 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>41</v>
-      </c>
+      <c r="C10" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -717,6 +730,7 @@
     <hyperlink ref="C2" r:id="rId1" xr:uid="{DCED2FB3-3551-4673-8C13-23B6281785A3}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{78B9E718-AD38-4C81-A2B6-E5AC60DFB2F4}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{900FE156-2E37-48CB-995D-825E3E8DE055}"/>
+    <hyperlink ref="C9" r:id="rId4" xr:uid="{4400B83A-4007-46D7-943D-71DE4B8C0A00}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -724,10 +738,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB75600-C524-4091-8455-43029D226ECA}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -738,9 +752,10 @@
     <col min="6" max="6" width="12.796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.59765625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -765,8 +780,11 @@
       <c r="H1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -789,7 +807,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -800,7 +818,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -811,7 +829,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -819,7 +837,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -833,15 +851,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>24</v>
       </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
       <c r="E7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -855,7 +876,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>37</v>
       </c>

</xml_diff>